<commit_message>
Fixing the figure formats
</commit_message>
<xml_diff>
--- a/paper/data/no-interleaved/8node-no-interleaved.xlsx
+++ b/paper/data/no-interleaved/8node-no-interleaved.xlsx
@@ -1,20 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xinzhao/Desktop/data/no-interleaved/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tongpingliu/projects/numalloc/paper/data/no-interleaved/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F1CF9F-8D45-FA40-AFD1-6BBB28AF0546}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F267B15B-5EB2-0345-A8B5-3F3DCD06CA4A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-1940" windowWidth="38400" windowHeight="21600" xr2:uid="{3A2DC044-6BB7-684C-8FBF-8D134127710A}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16000" activeTab="1" xr2:uid="{3A2DC044-6BB7-684C-8FBF-8D134127710A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="2-Node" sheetId="2" r:id="rId1"/>
+    <sheet name="8Node" sheetId="1" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">'8Node'!$F$24:$F$36</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'8Node'!$G$23</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'8Node'!$G$24:$G$36</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'8Node'!$H$23</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">'8Node'!$H$24:$H$36</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -23,9 +31,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="29">
   <si>
     <t>pthread</t>
   </si>
@@ -114,6 +120,12 @@
   </si>
   <si>
     <t>numalloc-nointerleaved</t>
+  </si>
+  <si>
+    <t>W/O Interleaved Heap</t>
+  </si>
+  <si>
+    <t>With Interleaved Heap</t>
   </si>
 </sst>
 </file>
@@ -289,6 +301,1226 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.3997594050743654E-2"/>
+          <c:y val="0.16203703703703703"/>
+          <c:w val="0.89655796150481193"/>
+          <c:h val="0.58385644502770484"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'8Node'!$G$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>With Interleaved Heap</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="pct30">
+              <a:fgClr>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="85000"/>
+                  <a:lumOff val="15000"/>
+                </a:schemeClr>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg1"/>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'8Node'!$F$24:$F$36</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>aget</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>canneal</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>dedup</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>fluidanimate</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>raytrace</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>vips</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>aget</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>canneal</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>dedup</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>fluidanimate</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>raytrace</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>vips</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'8Node'!$G$24:$G$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0449999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.97499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.96499999999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.2050000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.93500000000000005</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0507177041148326</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.2820669671603346</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.75308642001151072</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.1721445104156184</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.1093101858964509</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.96641007697690706</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F2F2-3148-8BE6-A660123B83EE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'8Node'!$H$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>W/O Interleaved Heap</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="pct60">
+              <a:fgClr>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="85000"/>
+                  <a:lumOff val="15000"/>
+                </a:schemeClr>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg1"/>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'8Node'!$F$24:$F$36</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>aget</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>canneal</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>dedup</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>fluidanimate</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>raytrace</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>vips</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>aget</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>canneal</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>dedup</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>fluidanimate</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>raytrace</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>vips</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'8Node'!$H$24:$H$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.97699999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.97499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.93</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.95499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.9395</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.2172248802679426</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.75022537024855107</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.87377925204993978</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.55757270805595249</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.87548010446919644</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.86958890839256531</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F2F2-3148-8BE6-A660123B83EE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:axId val="1425530319"/>
+        <c:axId val="1425532591"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1425530319"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1425532591"/>
+        <c:crossesAt val="0"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="1"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1425532591"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Normalized Runtime</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0"/>
+              <c:y val="0.21196295054961017"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1425530319"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.22286392436178287"/>
+          <c:y val="9.123987841763001E-2"/>
+          <c:w val="0.55427215127643426"/>
+          <c:h val="6.69427706374391E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>375739</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>501236</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>157960</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4CC978DB-A526-C747-91C8-ACAB78438B1B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>315622</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>127751</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>75147</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>172840</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{345EF61A-56C9-6841-B1E3-A19AB73B7CD2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6928640" y="2968343"/>
+          <a:ext cx="3892661" cy="247988"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Machine A (2-Node)                                       Machine B (8-Node)</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -587,11 +1819,1556 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E52C62D-7A23-7E4D-81E0-AC790BE30E7F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6A5AD0A-0C27-F54D-AEFC-8A9BB49D28C7}">
   <dimension ref="A1:H110"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="169" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D24"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4">
+        <v>18.697500000000002</v>
+      </c>
+      <c r="C2" s="4">
+        <v>18.181249999999999</v>
+      </c>
+      <c r="D2" s="4">
+        <v>18.4449999998</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="4">
+        <v>10.69125</v>
+      </c>
+      <c r="C3" s="4">
+        <v>10.141249999999999</v>
+      </c>
+      <c r="D3" s="4">
+        <v>10.143750000700001</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="4">
+        <v>28.88</v>
+      </c>
+      <c r="C4" s="4">
+        <v>30.1875</v>
+      </c>
+      <c r="D4" s="4">
+        <v>25.339999999900002</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="4">
+        <v>12.83625</v>
+      </c>
+      <c r="C5" s="4">
+        <v>12.52125</v>
+      </c>
+      <c r="D5" s="4">
+        <v>12.5175000001</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="4">
+        <v>156.3075</v>
+      </c>
+      <c r="C6" s="4">
+        <v>163.82</v>
+      </c>
+      <c r="D6" s="4">
+        <v>163.66499999999999</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="4">
+        <v>24.096250000000001</v>
+      </c>
+      <c r="C7" s="4">
+        <v>25.605</v>
+      </c>
+      <c r="D7" s="4">
+        <v>25.528750000100001</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="4">
+        <v>13.425000000000001</v>
+      </c>
+      <c r="C8" s="4">
+        <v>11.61875</v>
+      </c>
+      <c r="D8" s="4">
+        <v>12.4312500004</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="4">
+        <v>40.28125</v>
+      </c>
+      <c r="C9" s="4">
+        <v>48.541249999999998</v>
+      </c>
+      <c r="D9" s="4">
+        <v>34.463750000099999</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="4">
+        <v>23.916250000000002</v>
+      </c>
+      <c r="C10" s="4">
+        <v>21.087499999999999</v>
+      </c>
+      <c r="D10" s="4">
+        <v>24.495000000600001</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="4">
+        <v>14.4925</v>
+      </c>
+      <c r="C11" s="4">
+        <v>14.42375</v>
+      </c>
+      <c r="D11" s="4">
+        <v>14.436250000299999</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="4">
+        <v>16.88</v>
+      </c>
+      <c r="C12" s="4">
+        <v>15.79125</v>
+      </c>
+      <c r="D12" s="4">
+        <v>15.859999999899999</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="4">
+        <v>24.46875</v>
+      </c>
+      <c r="C13" s="4">
+        <v>22.445</v>
+      </c>
+      <c r="D13" s="4">
+        <v>22.2675000001</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="4">
+        <v>2.92625</v>
+      </c>
+      <c r="C14" s="4">
+        <v>2.9787499999999998</v>
+      </c>
+      <c r="D14" s="4">
+        <v>2.8799999998899999</v>
+      </c>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="4">
+        <v>2.3462499999999999</v>
+      </c>
+      <c r="C15" s="4">
+        <v>1.5475000000000001</v>
+      </c>
+      <c r="D15" s="4">
+        <v>1.57250000024</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="4">
+        <v>435.99624999999997</v>
+      </c>
+      <c r="C16" s="4">
+        <v>425.60500000000002</v>
+      </c>
+      <c r="D16" s="4">
+        <v>726.83</v>
+      </c>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="4">
+        <v>70.52</v>
+      </c>
+      <c r="C17" s="4">
+        <v>70.097499999999997</v>
+      </c>
+      <c r="D17" s="4">
+        <v>69.886250000000004</v>
+      </c>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="8">
+        <v>57.241999999999997</v>
+      </c>
+      <c r="C18" s="8">
+        <v>60.991</v>
+      </c>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="8">
+        <v>9.8160000000000007</v>
+      </c>
+      <c r="C19" s="8">
+        <v>8.734</v>
+      </c>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="9">
+        <v>221.84</v>
+      </c>
+      <c r="C20" s="9">
+        <v>220.13800000000001</v>
+      </c>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="11"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="4">
+        <v>2.67875</v>
+      </c>
+      <c r="C21" s="4">
+        <v>0.40874999989999999</v>
+      </c>
+      <c r="D21" s="4">
+        <v>2.4475000002399998</v>
+      </c>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="4">
+        <v>2.55125</v>
+      </c>
+      <c r="C22" s="4">
+        <v>2.5274999999999999</v>
+      </c>
+      <c r="D22" s="4">
+        <v>2.4725000006100002</v>
+      </c>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="4">
+        <v>7.3250000000000002</v>
+      </c>
+      <c r="C23" s="4">
+        <v>1.44625</v>
+      </c>
+      <c r="D23" s="4">
+        <v>1.4375</v>
+      </c>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="4">
+        <v>207325436</v>
+      </c>
+      <c r="C24" s="4">
+        <v>360670607</v>
+      </c>
+      <c r="D24" s="4">
+        <v>366212483</v>
+      </c>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" s="1"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B30" s="1">
+        <v>1</v>
+      </c>
+      <c r="C30" s="4">
+        <f>C2/B2</f>
+        <v>0.97238935686589101</v>
+      </c>
+      <c r="D30" s="4">
+        <f>D2/B2</f>
+        <v>0.98649552078085301</v>
+      </c>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31" s="4">
+        <v>1</v>
+      </c>
+      <c r="C31" s="4">
+        <f t="shared" ref="C31:C50" si="0">C3/B3</f>
+        <v>0.94855606220039745</v>
+      </c>
+      <c r="D31" s="4">
+        <f>D3/B3</f>
+        <v>0.94878989834677896</v>
+      </c>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" s="17">
+        <v>1</v>
+      </c>
+      <c r="C32" s="17">
+        <f t="shared" si="0"/>
+        <v>1.0452735457063713</v>
+      </c>
+      <c r="D32" s="17">
+        <f t="shared" ref="D32:D53" si="1">D4/B4</f>
+        <v>0.87742382271121888</v>
+      </c>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" s="4">
+        <v>1</v>
+      </c>
+      <c r="C33" s="4">
+        <f t="shared" si="0"/>
+        <v>0.97546012269938653</v>
+      </c>
+      <c r="D33" s="4">
+        <f t="shared" si="1"/>
+        <v>0.97516798131074112</v>
+      </c>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" s="4">
+        <v>1</v>
+      </c>
+      <c r="C34" s="4">
+        <f t="shared" si="0"/>
+        <v>1.0480623130687907</v>
+      </c>
+      <c r="D34" s="4">
+        <f t="shared" si="1"/>
+        <v>1.0470706779904995</v>
+      </c>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" s="4">
+        <v>1</v>
+      </c>
+      <c r="C35" s="4">
+        <f t="shared" si="0"/>
+        <v>1.0626134772008091</v>
+      </c>
+      <c r="D35" s="4">
+        <f t="shared" si="1"/>
+        <v>1.0594490844052498</v>
+      </c>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36" s="17">
+        <v>1</v>
+      </c>
+      <c r="C36" s="17">
+        <f t="shared" si="0"/>
+        <v>0.86545623836126628</v>
+      </c>
+      <c r="D36" s="17">
+        <f t="shared" si="1"/>
+        <v>0.92597765366108009</v>
+      </c>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B37" s="17">
+        <v>1</v>
+      </c>
+      <c r="C37" s="17">
+        <f t="shared" si="0"/>
+        <v>1.2050581846392552</v>
+      </c>
+      <c r="D37" s="17">
+        <f t="shared" si="1"/>
+        <v>0.85557796741908454</v>
+      </c>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B38" s="17">
+        <v>1</v>
+      </c>
+      <c r="C38" s="17">
+        <f t="shared" si="0"/>
+        <v>0.88172267809543714</v>
+      </c>
+      <c r="D38" s="17">
+        <f t="shared" si="1"/>
+        <v>1.0241990278827158</v>
+      </c>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B39" s="4">
+        <v>1</v>
+      </c>
+      <c r="C39" s="4">
+        <f t="shared" si="0"/>
+        <v>0.99525616698292219</v>
+      </c>
+      <c r="D39" s="4">
+        <f t="shared" si="1"/>
+        <v>0.99611868209763665</v>
+      </c>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40" s="4">
+        <v>1</v>
+      </c>
+      <c r="C40" s="4">
+        <f t="shared" si="0"/>
+        <v>0.93550059241706163</v>
+      </c>
+      <c r="D40" s="4">
+        <f t="shared" si="1"/>
+        <v>0.93957345970971562</v>
+      </c>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4"/>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B41" s="4">
+        <v>1</v>
+      </c>
+      <c r="C41" s="4">
+        <f t="shared" si="0"/>
+        <v>0.91729246487867178</v>
+      </c>
+      <c r="D41" s="4">
+        <f t="shared" si="1"/>
+        <v>0.9100383141803321</v>
+      </c>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B42" s="4">
+        <v>1</v>
+      </c>
+      <c r="C42" s="4">
+        <f t="shared" si="0"/>
+        <v>1.0179410508329774</v>
+      </c>
+      <c r="D42" s="4">
+        <f t="shared" si="1"/>
+        <v>0.98419478851431008</v>
+      </c>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B43" s="4">
+        <v>1</v>
+      </c>
+      <c r="C43" s="4">
+        <f t="shared" si="0"/>
+        <v>0.65956313265849764</v>
+      </c>
+      <c r="D43" s="4">
+        <f t="shared" si="1"/>
+        <v>0.67021843377304213</v>
+      </c>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4"/>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B44" s="4">
+        <v>1</v>
+      </c>
+      <c r="C44" s="4">
+        <f t="shared" si="0"/>
+        <v>0.97616665280951398</v>
+      </c>
+      <c r="D44" s="4">
+        <f t="shared" si="1"/>
+        <v>1.6670556226114333</v>
+      </c>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
+      <c r="H44" s="4"/>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B45" s="4">
+        <v>1</v>
+      </c>
+      <c r="C45" s="4">
+        <f t="shared" si="0"/>
+        <v>0.99400879183210433</v>
+      </c>
+      <c r="D45" s="4">
+        <f t="shared" si="1"/>
+        <v>0.99101318774815661</v>
+      </c>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4"/>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B46" s="4">
+        <v>1</v>
+      </c>
+      <c r="C46" s="4">
+        <f t="shared" si="0"/>
+        <v>1.0654938681387793</v>
+      </c>
+      <c r="D46" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
+      <c r="H46" s="4"/>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B47" s="4">
+        <v>1</v>
+      </c>
+      <c r="C47" s="4">
+        <f t="shared" si="0"/>
+        <v>0.88977180114099419</v>
+      </c>
+      <c r="D47" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
+      <c r="H47" s="4"/>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B48" s="4">
+        <v>1</v>
+      </c>
+      <c r="C48" s="4">
+        <f t="shared" si="0"/>
+        <v>0.99232780382257479</v>
+      </c>
+      <c r="D48" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="4"/>
+      <c r="H48" s="4"/>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B49" s="4">
+        <v>1</v>
+      </c>
+      <c r="C49" s="4">
+        <f t="shared" si="0"/>
+        <v>0.15258982730751283</v>
+      </c>
+      <c r="D49" s="4">
+        <f t="shared" si="1"/>
+        <v>0.91367242192813802</v>
+      </c>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
+      <c r="H49" s="4"/>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B50" s="4">
+        <v>1</v>
+      </c>
+      <c r="C50" s="4">
+        <f t="shared" si="0"/>
+        <v>0.99069083782459577</v>
+      </c>
+      <c r="D50" s="4">
+        <f t="shared" si="1"/>
+        <v>0.96913277828907407</v>
+      </c>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
+      <c r="H50" s="4"/>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B51" s="4">
+        <v>1</v>
+      </c>
+      <c r="C51" s="4">
+        <f>C23/B23</f>
+        <v>0.19744027303754266</v>
+      </c>
+      <c r="D51" s="4">
+        <f t="shared" si="1"/>
+        <v>0.19624573378839591</v>
+      </c>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
+      <c r="G51" s="4"/>
+      <c r="H51" s="4"/>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B52" s="4">
+        <v>1</v>
+      </c>
+      <c r="C52" s="4">
+        <f>B24/C24</f>
+        <v>0.57483319121704868</v>
+      </c>
+      <c r="D52" s="4">
+        <f>B24/D24</f>
+        <v>0.56613426801183075</v>
+      </c>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
+      <c r="G52" s="4"/>
+      <c r="H52" s="4"/>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B53" s="12">
+        <v>1</v>
+      </c>
+      <c r="C53" s="4">
+        <f>SUM(C30:C52)/23</f>
+        <v>0.88536819277123502</v>
+      </c>
+      <c r="D53" s="4" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E53" s="12"/>
+      <c r="F53" s="12"/>
+      <c r="G53" s="12"/>
+      <c r="H53" s="12"/>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" s="12"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="1"/>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1"/>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="1"/>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="A59" s="12"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="2"/>
+      <c r="G59" s="1"/>
+      <c r="H59" s="1"/>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="A60" s="3"/>
+      <c r="B60" s="4"/>
+      <c r="C60" s="4"/>
+      <c r="D60" s="4"/>
+      <c r="E60" s="4"/>
+      <c r="F60" s="4"/>
+      <c r="G60" s="4"/>
+      <c r="H60" s="4"/>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="A61" s="5"/>
+      <c r="B61" s="4"/>
+      <c r="C61" s="4"/>
+      <c r="D61" s="4"/>
+      <c r="E61" s="4"/>
+      <c r="F61" s="4"/>
+      <c r="G61" s="4"/>
+      <c r="H61" s="4"/>
+    </row>
+    <row r="62" spans="1:8">
+      <c r="A62" s="3"/>
+      <c r="B62" s="4"/>
+      <c r="C62" s="4"/>
+      <c r="D62" s="4"/>
+      <c r="E62" s="4"/>
+      <c r="F62" s="4"/>
+      <c r="G62" s="4"/>
+      <c r="H62" s="4"/>
+    </row>
+    <row r="63" spans="1:8">
+      <c r="A63" s="5"/>
+      <c r="B63" s="4"/>
+      <c r="C63" s="4"/>
+      <c r="D63" s="4"/>
+      <c r="E63" s="4"/>
+      <c r="F63" s="4"/>
+      <c r="G63" s="4"/>
+      <c r="H63" s="4"/>
+    </row>
+    <row r="64" spans="1:8">
+      <c r="A64" s="5"/>
+      <c r="B64" s="4"/>
+      <c r="C64" s="4"/>
+      <c r="D64" s="4"/>
+      <c r="E64" s="4"/>
+      <c r="F64" s="4"/>
+      <c r="G64" s="4"/>
+      <c r="H64" s="4"/>
+    </row>
+    <row r="65" spans="1:8">
+      <c r="A65" s="5"/>
+      <c r="B65" s="4"/>
+      <c r="C65" s="4"/>
+      <c r="D65" s="4"/>
+      <c r="E65" s="4"/>
+      <c r="F65" s="4"/>
+      <c r="G65" s="4"/>
+      <c r="H65" s="4"/>
+    </row>
+    <row r="66" spans="1:8">
+      <c r="A66" s="3"/>
+      <c r="B66" s="4"/>
+      <c r="C66" s="4"/>
+      <c r="D66" s="4"/>
+      <c r="E66" s="4"/>
+      <c r="F66" s="4"/>
+      <c r="G66" s="4"/>
+      <c r="H66" s="4"/>
+    </row>
+    <row r="67" spans="1:8">
+      <c r="A67" s="5"/>
+      <c r="B67" s="4"/>
+      <c r="C67" s="4"/>
+      <c r="D67" s="4"/>
+      <c r="E67" s="4"/>
+      <c r="F67" s="4"/>
+      <c r="G67" s="4"/>
+      <c r="H67" s="4"/>
+    </row>
+    <row r="68" spans="1:8">
+      <c r="A68" s="3"/>
+      <c r="B68" s="4"/>
+      <c r="C68" s="4"/>
+      <c r="D68" s="4"/>
+      <c r="E68" s="4"/>
+      <c r="F68" s="4"/>
+      <c r="G68" s="4"/>
+      <c r="H68" s="4"/>
+    </row>
+    <row r="69" spans="1:8">
+      <c r="A69" s="3"/>
+      <c r="B69" s="4"/>
+      <c r="C69" s="4"/>
+      <c r="D69" s="4"/>
+      <c r="E69" s="4"/>
+      <c r="F69" s="4"/>
+      <c r="G69" s="4"/>
+      <c r="H69" s="4"/>
+    </row>
+    <row r="70" spans="1:8">
+      <c r="A70" s="5"/>
+      <c r="B70" s="4"/>
+      <c r="C70" s="4"/>
+      <c r="D70" s="4"/>
+      <c r="E70" s="4"/>
+      <c r="F70" s="4"/>
+      <c r="G70" s="4"/>
+      <c r="H70" s="4"/>
+    </row>
+    <row r="71" spans="1:8">
+      <c r="A71" s="3"/>
+      <c r="B71" s="4"/>
+      <c r="C71" s="4"/>
+      <c r="D71" s="4"/>
+      <c r="E71" s="4"/>
+      <c r="F71" s="4"/>
+      <c r="G71" s="4"/>
+      <c r="H71" s="4"/>
+    </row>
+    <row r="72" spans="1:8">
+      <c r="A72" s="6"/>
+      <c r="B72" s="4"/>
+      <c r="C72" s="4"/>
+      <c r="D72" s="4"/>
+      <c r="E72" s="4"/>
+      <c r="F72" s="4"/>
+      <c r="G72" s="4"/>
+      <c r="H72" s="4"/>
+    </row>
+    <row r="73" spans="1:8">
+      <c r="A73" s="7"/>
+      <c r="B73" s="4"/>
+      <c r="C73" s="4"/>
+      <c r="D73" s="4"/>
+      <c r="E73" s="4"/>
+      <c r="F73" s="4"/>
+      <c r="G73" s="4"/>
+      <c r="H73" s="4"/>
+    </row>
+    <row r="74" spans="1:8">
+      <c r="A74" s="7"/>
+      <c r="B74" s="4"/>
+      <c r="C74" s="4"/>
+      <c r="D74" s="4"/>
+      <c r="E74" s="4"/>
+      <c r="F74" s="4"/>
+      <c r="G74" s="4"/>
+      <c r="H74" s="4"/>
+    </row>
+    <row r="75" spans="1:8">
+      <c r="A75" s="7"/>
+      <c r="B75" s="4"/>
+      <c r="C75" s="4"/>
+      <c r="D75" s="4"/>
+      <c r="E75" s="4"/>
+      <c r="F75" s="4"/>
+      <c r="G75" s="4"/>
+      <c r="H75" s="4"/>
+    </row>
+    <row r="76" spans="1:8">
+      <c r="A76" s="1"/>
+      <c r="B76" s="8"/>
+      <c r="C76" s="1"/>
+      <c r="D76" s="1"/>
+      <c r="E76" s="1"/>
+      <c r="F76" s="5"/>
+      <c r="G76" s="1"/>
+      <c r="H76" s="1"/>
+    </row>
+    <row r="77" spans="1:8">
+      <c r="A77" s="1"/>
+      <c r="B77" s="1"/>
+      <c r="C77" s="1"/>
+      <c r="D77" s="1"/>
+      <c r="E77" s="1"/>
+      <c r="F77" s="5"/>
+      <c r="G77" s="1"/>
+      <c r="H77" s="1"/>
+    </row>
+    <row r="78" spans="1:8">
+      <c r="A78" s="1"/>
+      <c r="B78" s="1"/>
+      <c r="C78" s="1"/>
+      <c r="D78" s="1"/>
+      <c r="E78" s="1"/>
+      <c r="F78" s="5"/>
+      <c r="G78" s="1"/>
+      <c r="H78" s="13"/>
+    </row>
+    <row r="79" spans="1:8">
+      <c r="A79" s="4"/>
+      <c r="B79" s="4"/>
+      <c r="C79" s="4"/>
+      <c r="D79" s="4"/>
+      <c r="E79" s="4"/>
+      <c r="F79" s="4"/>
+      <c r="G79" s="4"/>
+      <c r="H79" s="4"/>
+    </row>
+    <row r="80" spans="1:8">
+      <c r="A80" s="4"/>
+      <c r="B80" s="4"/>
+      <c r="C80" s="4"/>
+      <c r="D80" s="4"/>
+      <c r="E80" s="4"/>
+      <c r="F80" s="4"/>
+      <c r="G80" s="4"/>
+      <c r="H80" s="4"/>
+    </row>
+    <row r="81" spans="1:8">
+      <c r="A81" s="4"/>
+      <c r="B81" s="4"/>
+      <c r="C81" s="4"/>
+      <c r="D81" s="4"/>
+      <c r="E81" s="4"/>
+      <c r="F81" s="4"/>
+      <c r="G81" s="4"/>
+      <c r="H81" s="4"/>
+    </row>
+    <row r="82" spans="1:8">
+      <c r="A82" s="4"/>
+      <c r="B82" s="4"/>
+      <c r="C82" s="4"/>
+      <c r="D82" s="4"/>
+      <c r="E82" s="4"/>
+      <c r="F82" s="4"/>
+      <c r="G82" s="4"/>
+      <c r="H82" s="4"/>
+    </row>
+    <row r="83" spans="1:8">
+      <c r="A83" s="1"/>
+      <c r="B83" s="1"/>
+      <c r="C83" s="1"/>
+      <c r="D83" s="1"/>
+      <c r="E83" s="1"/>
+      <c r="F83" s="1"/>
+      <c r="G83" s="1"/>
+      <c r="H83" s="1"/>
+    </row>
+    <row r="84" spans="1:8">
+      <c r="A84" s="1"/>
+      <c r="B84" s="1"/>
+      <c r="C84" s="1"/>
+      <c r="D84" s="1"/>
+      <c r="E84" s="1"/>
+      <c r="F84" s="1"/>
+      <c r="G84" s="1"/>
+      <c r="H84" s="1"/>
+    </row>
+    <row r="85" spans="1:8">
+      <c r="A85" s="14"/>
+      <c r="B85" s="1"/>
+      <c r="C85" s="1"/>
+      <c r="D85" s="1"/>
+      <c r="E85" s="1"/>
+      <c r="F85" s="2"/>
+      <c r="G85" s="1"/>
+      <c r="H85" s="1"/>
+    </row>
+    <row r="86" spans="1:8">
+      <c r="A86" s="3"/>
+      <c r="B86" s="4"/>
+      <c r="C86" s="4"/>
+      <c r="D86" s="4"/>
+      <c r="E86" s="4"/>
+      <c r="F86" s="4"/>
+      <c r="G86" s="4"/>
+      <c r="H86" s="4"/>
+    </row>
+    <row r="87" spans="1:8">
+      <c r="A87" s="5"/>
+      <c r="B87" s="4"/>
+      <c r="C87" s="4"/>
+      <c r="D87" s="4"/>
+      <c r="E87" s="4"/>
+      <c r="F87" s="4"/>
+      <c r="G87" s="4"/>
+      <c r="H87" s="4"/>
+    </row>
+    <row r="88" spans="1:8">
+      <c r="A88" s="3"/>
+      <c r="B88" s="4"/>
+      <c r="C88" s="4"/>
+      <c r="D88" s="4"/>
+      <c r="E88" s="4"/>
+      <c r="F88" s="4"/>
+      <c r="G88" s="4"/>
+      <c r="H88" s="4"/>
+    </row>
+    <row r="89" spans="1:8">
+      <c r="A89" s="5"/>
+      <c r="B89" s="4"/>
+      <c r="C89" s="4"/>
+      <c r="D89" s="4"/>
+      <c r="E89" s="4"/>
+      <c r="F89" s="4"/>
+      <c r="G89" s="4"/>
+      <c r="H89" s="4"/>
+    </row>
+    <row r="90" spans="1:8">
+      <c r="A90" s="5"/>
+      <c r="B90" s="4"/>
+      <c r="C90" s="4"/>
+      <c r="D90" s="4"/>
+      <c r="E90" s="4"/>
+      <c r="F90" s="4"/>
+      <c r="G90" s="4"/>
+      <c r="H90" s="4"/>
+    </row>
+    <row r="91" spans="1:8">
+      <c r="A91" s="5"/>
+      <c r="B91" s="4"/>
+      <c r="C91" s="4"/>
+      <c r="D91" s="4"/>
+      <c r="E91" s="4"/>
+      <c r="F91" s="4"/>
+      <c r="G91" s="4"/>
+      <c r="H91" s="4"/>
+    </row>
+    <row r="92" spans="1:8">
+      <c r="A92" s="3"/>
+      <c r="B92" s="4"/>
+      <c r="C92" s="4"/>
+      <c r="D92" s="4"/>
+      <c r="E92" s="4"/>
+      <c r="F92" s="4"/>
+      <c r="G92" s="4"/>
+      <c r="H92" s="4"/>
+    </row>
+    <row r="93" spans="1:8">
+      <c r="A93" s="5"/>
+      <c r="B93" s="4"/>
+      <c r="C93" s="4"/>
+      <c r="D93" s="4"/>
+      <c r="E93" s="4"/>
+      <c r="F93" s="4"/>
+      <c r="G93" s="4"/>
+      <c r="H93" s="4"/>
+    </row>
+    <row r="94" spans="1:8">
+      <c r="A94" s="3"/>
+      <c r="B94" s="4"/>
+      <c r="C94" s="4"/>
+      <c r="D94" s="4"/>
+      <c r="E94" s="4"/>
+      <c r="F94" s="4"/>
+      <c r="G94" s="4"/>
+      <c r="H94" s="4"/>
+    </row>
+    <row r="95" spans="1:8">
+      <c r="A95" s="3"/>
+      <c r="B95" s="4"/>
+      <c r="C95" s="4"/>
+      <c r="D95" s="4"/>
+      <c r="E95" s="4"/>
+      <c r="F95" s="4"/>
+      <c r="G95" s="4"/>
+      <c r="H95" s="4"/>
+    </row>
+    <row r="96" spans="1:8">
+      <c r="A96" s="5"/>
+      <c r="B96" s="4"/>
+      <c r="C96" s="4"/>
+      <c r="D96" s="4"/>
+      <c r="E96" s="4"/>
+      <c r="F96" s="4"/>
+      <c r="G96" s="4"/>
+      <c r="H96" s="4"/>
+    </row>
+    <row r="97" spans="1:8">
+      <c r="A97" s="3"/>
+      <c r="B97" s="4"/>
+      <c r="C97" s="4"/>
+      <c r="D97" s="4"/>
+      <c r="E97" s="4"/>
+      <c r="F97" s="4"/>
+      <c r="G97" s="4"/>
+      <c r="H97" s="4"/>
+    </row>
+    <row r="98" spans="1:8">
+      <c r="A98" s="6"/>
+      <c r="B98" s="4"/>
+      <c r="C98" s="4"/>
+      <c r="D98" s="4"/>
+      <c r="E98" s="4"/>
+      <c r="F98" s="4"/>
+      <c r="G98" s="4"/>
+      <c r="H98" s="4"/>
+    </row>
+    <row r="99" spans="1:8">
+      <c r="A99" s="7"/>
+      <c r="B99" s="4"/>
+      <c r="C99" s="4"/>
+      <c r="D99" s="4"/>
+      <c r="E99" s="4"/>
+      <c r="F99" s="4"/>
+      <c r="G99" s="4"/>
+      <c r="H99" s="4"/>
+    </row>
+    <row r="100" spans="1:8">
+      <c r="A100" s="7"/>
+      <c r="B100" s="4"/>
+      <c r="C100" s="4"/>
+      <c r="D100" s="4"/>
+      <c r="E100" s="4"/>
+      <c r="F100" s="4"/>
+      <c r="G100" s="4"/>
+      <c r="H100" s="4"/>
+    </row>
+    <row r="101" spans="1:8">
+      <c r="A101" s="7"/>
+      <c r="B101" s="4"/>
+      <c r="C101" s="4"/>
+      <c r="D101" s="4"/>
+      <c r="E101" s="4"/>
+      <c r="F101" s="4"/>
+      <c r="G101" s="4"/>
+      <c r="H101" s="4"/>
+    </row>
+    <row r="102" spans="1:8">
+      <c r="A102" s="1"/>
+      <c r="B102" s="4"/>
+      <c r="C102" s="4"/>
+      <c r="D102" s="4"/>
+      <c r="E102" s="4"/>
+      <c r="F102" s="4"/>
+      <c r="G102" s="4"/>
+      <c r="H102" s="4"/>
+    </row>
+    <row r="103" spans="1:8">
+      <c r="A103" s="1"/>
+      <c r="B103" s="4"/>
+      <c r="C103" s="4"/>
+      <c r="D103" s="4"/>
+      <c r="E103" s="4"/>
+      <c r="F103" s="4"/>
+      <c r="G103" s="4"/>
+      <c r="H103" s="4"/>
+    </row>
+    <row r="104" spans="1:8">
+      <c r="A104" s="15"/>
+      <c r="B104" s="4"/>
+      <c r="C104" s="4"/>
+      <c r="D104" s="4"/>
+      <c r="E104" s="4"/>
+      <c r="F104" s="4"/>
+      <c r="G104" s="4"/>
+      <c r="H104" s="4"/>
+    </row>
+    <row r="105" spans="1:8">
+      <c r="A105" s="15"/>
+      <c r="B105" s="4"/>
+      <c r="C105" s="4"/>
+      <c r="D105" s="4"/>
+      <c r="E105" s="4"/>
+      <c r="F105" s="4"/>
+      <c r="G105" s="4"/>
+      <c r="H105" s="4"/>
+    </row>
+    <row r="106" spans="1:8">
+      <c r="A106" s="4"/>
+      <c r="B106" s="4"/>
+      <c r="C106" s="4"/>
+      <c r="D106" s="4"/>
+      <c r="E106" s="4"/>
+      <c r="F106" s="4"/>
+      <c r="G106" s="4"/>
+      <c r="H106" s="4"/>
+    </row>
+    <row r="107" spans="1:8">
+      <c r="A107" s="4"/>
+      <c r="B107" s="4"/>
+      <c r="C107" s="4"/>
+      <c r="D107" s="4"/>
+      <c r="E107" s="4"/>
+      <c r="F107" s="4"/>
+      <c r="G107" s="4"/>
+      <c r="H107" s="4"/>
+    </row>
+    <row r="108" spans="1:8">
+      <c r="A108" s="4"/>
+      <c r="B108" s="4"/>
+      <c r="C108" s="4"/>
+      <c r="D108" s="4"/>
+      <c r="E108" s="4"/>
+      <c r="F108" s="4"/>
+      <c r="G108" s="4"/>
+      <c r="H108" s="4"/>
+    </row>
+    <row r="109" spans="1:8">
+      <c r="A109" s="4"/>
+      <c r="B109" s="4"/>
+      <c r="C109" s="4"/>
+      <c r="D109" s="4"/>
+      <c r="E109" s="4"/>
+      <c r="F109" s="4"/>
+      <c r="G109" s="4"/>
+      <c r="H109" s="4"/>
+    </row>
+    <row r="110" spans="1:8">
+      <c r="A110" s="12"/>
+      <c r="B110" s="1"/>
+      <c r="C110" s="1"/>
+      <c r="D110" s="1"/>
+      <c r="E110" s="1"/>
+      <c r="F110" s="1"/>
+      <c r="G110" s="1"/>
+      <c r="H110" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E52C62D-7A23-7E4D-81E0-AC790BE30E7F}">
+  <dimension ref="A1:H111"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="169" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1002,8 +3779,12 @@
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
+      <c r="G23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="4" t="s">
@@ -1019,9 +3800,15 @@
         <v>311127857</v>
       </c>
       <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
+      <c r="F24" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" s="4">
+        <v>1.01</v>
+      </c>
+      <c r="H24" s="4">
+        <v>0.98</v>
+      </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="1"/>
@@ -1029,9 +3816,15 @@
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
+      <c r="F25" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G25" s="1">
+        <v>1.0449999999999999</v>
+      </c>
+      <c r="H25" s="1">
+        <v>0.97699999999999998</v>
+      </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="1"/>
@@ -1039,9 +3832,15 @@
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
+      <c r="F26" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G26" s="1">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="H26" s="1">
+        <v>0.97499999999999998</v>
+      </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="1"/>
@@ -1049,9 +3848,15 @@
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
+      <c r="F27" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G27" s="1">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="H27" s="1">
+        <v>0.93</v>
+      </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="1"/>
@@ -1059,9 +3864,15 @@
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
+      <c r="F28" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G28" s="1">
+        <v>1.2050000000000001</v>
+      </c>
+      <c r="H28" s="1">
+        <v>0.95499999999999996</v>
+      </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="1"/>
@@ -1073,164 +3884,210 @@
         <v>26</v>
       </c>
       <c r="E29" s="1"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
+      <c r="F29" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G29" s="1">
+        <v>0.93500000000000005</v>
+      </c>
+      <c r="H29" s="1">
+        <v>0.9395</v>
+      </c>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="1">
-        <v>1</v>
-      </c>
-      <c r="C30" s="4">
+      <c r="B31" s="1">
+        <v>1</v>
+      </c>
+      <c r="C31" s="4">
         <f>C2/B2</f>
         <v>0.99633643718516263</v>
       </c>
-      <c r="D30" s="4">
+      <c r="D31" s="4">
         <f>D2/B2</f>
         <v>0.98453162364219204</v>
       </c>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-    </row>
-    <row r="31" spans="1:8">
-      <c r="A31" s="5" t="s">
+      <c r="E31" s="4"/>
+      <c r="F31" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G31" s="4">
+        <f>C43</f>
+        <v>1.0507177041148326</v>
+      </c>
+      <c r="H31" s="4">
+        <f>D43</f>
+        <v>1.2172248802679426</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B31" s="4">
-        <v>1</v>
-      </c>
-      <c r="C31" s="4">
-        <f t="shared" ref="C31:C51" si="0">C3/B3</f>
+      <c r="B32" s="4">
+        <v>1</v>
+      </c>
+      <c r="C32" s="4">
+        <f t="shared" ref="C32:C52" si="0">C3/B3</f>
         <v>1.0653719552337064</v>
       </c>
-      <c r="D31" s="4">
-        <f t="shared" ref="D31:D53" si="1">D3/B3</f>
+      <c r="D32" s="4">
+        <f t="shared" ref="D32:D54" si="1">D3/B3</f>
         <v>1.0680052666280448</v>
       </c>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-    </row>
-    <row r="32" spans="1:8">
-      <c r="A32" s="16" t="s">
+      <c r="E32" s="4"/>
+      <c r="F32" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B32" s="17">
-        <v>1</v>
-      </c>
-      <c r="C32" s="17">
+      <c r="G32" s="4">
+        <f>C33</f>
+        <v>1.2820669671603346</v>
+      </c>
+      <c r="H32" s="4">
+        <f>D33</f>
+        <v>0.75022537024855107</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" s="17">
+        <v>1</v>
+      </c>
+      <c r="C33" s="17">
         <f>C4/B4</f>
         <v>1.2820669671603346</v>
       </c>
-      <c r="D32" s="17">
+      <c r="D33" s="17">
         <f t="shared" si="1"/>
         <v>0.75022537024855107</v>
       </c>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-    </row>
-    <row r="33" spans="1:8">
-      <c r="A33" s="18" t="s">
+      <c r="E33" s="4"/>
+      <c r="F33" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B33" s="17">
-        <v>1</v>
-      </c>
-      <c r="C33" s="17">
+      <c r="G33" s="4">
+        <f>C34</f>
+        <v>0.75308642001151072</v>
+      </c>
+      <c r="H33" s="4">
+        <f>D34</f>
+        <v>0.87377925204993978</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="17">
+        <v>1</v>
+      </c>
+      <c r="C34" s="17">
         <f t="shared" si="0"/>
         <v>0.75308642001151072</v>
       </c>
-      <c r="D33" s="17">
+      <c r="D34" s="17">
         <f t="shared" si="1"/>
         <v>0.87377925204993978</v>
       </c>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
-    </row>
-    <row r="34" spans="1:8">
-      <c r="A34" s="5" t="s">
+      <c r="E34" s="4"/>
+      <c r="F34" s="4" t="str">
+        <f>A37</f>
+        <v>fluidanimate</v>
+      </c>
+      <c r="G34" s="4">
+        <f>C37</f>
+        <v>0.1721445104156184</v>
+      </c>
+      <c r="H34" s="4">
+        <f>D37</f>
+        <v>0.55757270805595249</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B34" s="4">
-        <v>1</v>
-      </c>
-      <c r="C34" s="4">
+      <c r="B35" s="4">
+        <v>1</v>
+      </c>
+      <c r="C35" s="4">
         <f t="shared" si="0"/>
         <v>0.98587553849097187</v>
       </c>
-      <c r="D34" s="4">
+      <c r="D35" s="4">
         <f t="shared" si="1"/>
         <v>0.96941569194028276</v>
       </c>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-    </row>
-    <row r="35" spans="1:8">
-      <c r="A35" s="5" t="s">
+      <c r="E35" s="4"/>
+      <c r="F35" s="4" t="str">
+        <f>A38</f>
+        <v>raytrace</v>
+      </c>
+      <c r="G35" s="4">
+        <f>C38</f>
+        <v>1.1093101858964509</v>
+      </c>
+      <c r="H35" s="4">
+        <f>D38</f>
+        <v>0.87548010446919644</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B35" s="4">
-        <v>1</v>
-      </c>
-      <c r="C35" s="4">
+      <c r="B36" s="4">
+        <v>1</v>
+      </c>
+      <c r="C36" s="4">
         <f>C7/B7</f>
         <v>0.99112244897959179</v>
       </c>
-      <c r="D35" s="4">
+      <c r="D36" s="4">
         <f t="shared" si="1"/>
         <v>0.98397959179591843</v>
       </c>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-    </row>
-    <row r="36" spans="1:8">
-      <c r="A36" s="16" t="s">
+      <c r="E36" s="4"/>
+      <c r="F36" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G36" s="4">
+        <f>C41</f>
+        <v>0.96641007697690706</v>
+      </c>
+      <c r="H36" s="4">
+        <f>D42</f>
+        <v>0.86958890839256531</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B36" s="17">
-        <v>1</v>
-      </c>
-      <c r="C36" s="17">
+      <c r="B37" s="17">
+        <v>1</v>
+      </c>
+      <c r="C37" s="17">
         <f t="shared" si="0"/>
         <v>0.1721445104156184</v>
       </c>
-      <c r="D36" s="17">
+      <c r="D37" s="17">
         <f t="shared" si="1"/>
         <v>0.55757270805595249</v>
-      </c>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-    </row>
-    <row r="37" spans="1:8">
-      <c r="A37" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="B37" s="17">
-        <v>1</v>
-      </c>
-      <c r="C37" s="17">
-        <f t="shared" si="0"/>
-        <v>1.1093101858964509</v>
-      </c>
-      <c r="D37" s="17">
-        <f t="shared" si="1"/>
-        <v>0.87548010446919644</v>
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
@@ -1238,19 +4095,19 @@
       <c r="H37" s="4"/>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B38" s="4">
-        <v>1</v>
-      </c>
-      <c r="C38" s="4">
+      <c r="A38" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B38" s="17">
+        <v>1</v>
+      </c>
+      <c r="C38" s="17">
         <f t="shared" si="0"/>
-        <v>0.6608883614478257</v>
-      </c>
-      <c r="D38" s="4">
+        <v>1.1093101858964509</v>
+      </c>
+      <c r="D38" s="17">
         <f t="shared" si="1"/>
-        <v>0.65898109687547679</v>
+        <v>0.87548010446919644</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
@@ -1259,18 +4116,18 @@
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B39" s="4">
         <v>1</v>
       </c>
       <c r="C39" s="4">
         <f t="shared" si="0"/>
-        <v>0.86177644670658682</v>
+        <v>0.6608883614478257</v>
       </c>
       <c r="D39" s="4">
         <f t="shared" si="1"/>
-        <v>0.85778443120558889</v>
+        <v>0.65898109687547679</v>
       </c>
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
@@ -1278,19 +4135,19 @@
       <c r="H39" s="4"/>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="5" t="s">
-        <v>12</v>
+      <c r="A40" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="B40" s="4">
         <v>1</v>
       </c>
       <c r="C40" s="4">
         <f t="shared" si="0"/>
-        <v>0.96641007697690706</v>
+        <v>0.86177644670658682</v>
       </c>
       <c r="D40" s="4">
         <f t="shared" si="1"/>
-        <v>1.0768019593603919</v>
+        <v>0.85778443120558889</v>
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
@@ -1298,19 +4155,19 @@
       <c r="H40" s="4"/>
     </row>
     <row r="41" spans="1:8">
-      <c r="A41" s="3" t="s">
-        <v>13</v>
+      <c r="A41" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="B41" s="4">
         <v>1</v>
       </c>
       <c r="C41" s="4">
         <f t="shared" si="0"/>
-        <v>0.892534963976509</v>
+        <v>0.96641007697690706</v>
       </c>
       <c r="D41" s="4">
         <f t="shared" si="1"/>
-        <v>0.86958890839256531</v>
+        <v>1.0768019593603919</v>
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
@@ -1318,19 +4175,19 @@
       <c r="H41" s="4"/>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="B42" s="17">
-        <v>1</v>
-      </c>
-      <c r="C42" s="17">
+      <c r="A42" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B42" s="4">
+        <v>1</v>
+      </c>
+      <c r="C42" s="4">
         <f t="shared" si="0"/>
-        <v>1.0507177041148326</v>
-      </c>
-      <c r="D42" s="17">
+        <v>0.892534963976509</v>
+      </c>
+      <c r="D42" s="4">
         <f t="shared" si="1"/>
-        <v>1.2172248802679426</v>
+        <v>0.86958890839256531</v>
       </c>
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
@@ -1338,19 +4195,19 @@
       <c r="H42" s="4"/>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B43" s="4">
-        <v>1</v>
-      </c>
-      <c r="C43" s="4">
+      <c r="A43" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B43" s="17">
+        <v>1</v>
+      </c>
+      <c r="C43" s="17">
         <f t="shared" si="0"/>
-        <v>0.70641389075741823</v>
-      </c>
-      <c r="D43" s="4">
+        <v>1.0507177041148326</v>
+      </c>
+      <c r="D43" s="17">
         <f t="shared" si="1"/>
-        <v>0.70854004232763435</v>
+        <v>1.2172248802679426</v>
       </c>
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
@@ -1359,18 +4216,18 @@
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B44" s="4">
         <v>1</v>
       </c>
       <c r="C44" s="4">
         <f t="shared" si="0"/>
-        <v>0.9888646142756361</v>
+        <v>0.70641389075741823</v>
       </c>
       <c r="D44" s="4">
         <f t="shared" si="1"/>
-        <v>0.98939755496377868</v>
+        <v>0.70854004232763435</v>
       </c>
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
@@ -1379,18 +4236,18 @@
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B45" s="4">
         <v>1</v>
       </c>
       <c r="C45" s="4">
         <f t="shared" si="0"/>
-        <v>0.9821656261902002</v>
+        <v>0.9888646142756361</v>
       </c>
       <c r="D45" s="4">
         <f t="shared" si="1"/>
-        <v>0.97820795178062236</v>
+        <v>0.98939755496377868</v>
       </c>
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
@@ -1398,19 +4255,19 @@
       <c r="H45" s="4"/>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" s="1" t="s">
-        <v>18</v>
+      <c r="A46" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="B46" s="4">
         <v>1</v>
       </c>
       <c r="C46" s="4">
         <f t="shared" si="0"/>
-        <v>1.025497512437811</v>
+        <v>0.9821656261902002</v>
       </c>
       <c r="D46" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.97820795178062236</v>
       </c>
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
@@ -1419,14 +4276,14 @@
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B47" s="4">
         <v>1</v>
       </c>
       <c r="C47" s="4">
         <f t="shared" si="0"/>
-        <v>1.0046522781774578</v>
+        <v>1.025497512437811</v>
       </c>
       <c r="D47" s="4">
         <f t="shared" si="1"/>
@@ -1439,14 +4296,14 @@
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B48" s="4">
         <v>1</v>
       </c>
       <c r="C48" s="4">
         <f t="shared" si="0"/>
-        <v>1.0280018468725387</v>
+        <v>1.0046522781774578</v>
       </c>
       <c r="D48" s="4">
         <f t="shared" si="1"/>
@@ -1458,19 +4315,19 @@
       <c r="H48" s="4"/>
     </row>
     <row r="49" spans="1:8">
-      <c r="A49" s="4" t="s">
-        <v>21</v>
+      <c r="A49" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="B49" s="4">
         <v>1</v>
       </c>
       <c r="C49" s="4">
         <f t="shared" si="0"/>
-        <v>7.7464788709424817E-2</v>
+        <v>1.0280018468725387</v>
       </c>
       <c r="D49" s="4">
         <f t="shared" si="1"/>
-        <v>7.4128984410932838E-2</v>
+        <v>0</v>
       </c>
       <c r="E49" s="4"/>
       <c r="F49" s="4"/>
@@ -1479,18 +4336,18 @@
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B50" s="4">
         <v>1</v>
       </c>
       <c r="C50" s="4">
         <f t="shared" si="0"/>
-        <v>0.77746478873239433</v>
+        <v>7.7464788709424817E-2</v>
       </c>
       <c r="D50" s="4">
         <f t="shared" si="1"/>
-        <v>0.77183098580281695</v>
+        <v>7.4128984410932838E-2</v>
       </c>
       <c r="E50" s="4"/>
       <c r="F50" s="4"/>
@@ -1499,18 +4356,18 @@
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B51" s="4">
         <v>1</v>
       </c>
       <c r="C51" s="4">
         <f t="shared" si="0"/>
-        <v>4.7430324735361802E-2</v>
+        <v>0.77746478873239433</v>
       </c>
       <c r="D51" s="4">
         <f t="shared" si="1"/>
-        <v>4.5768345716389672E-2</v>
+        <v>0.77183098580281695</v>
       </c>
       <c r="E51" s="4"/>
       <c r="F51" s="4"/>
@@ -1519,18 +4376,18 @@
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B52" s="4">
         <v>1</v>
       </c>
       <c r="C52" s="4">
-        <f>B24/C24</f>
-        <v>0.44395875172476118</v>
+        <f t="shared" si="0"/>
+        <v>4.7430324735361802E-2</v>
       </c>
       <c r="D52" s="4">
-        <f>B24/D24</f>
-        <v>0.45755785860087739</v>
+        <f t="shared" si="1"/>
+        <v>4.5768345716389672E-2</v>
       </c>
       <c r="E52" s="4"/>
       <c r="F52" s="4"/>
@@ -1538,36 +4395,46 @@
       <c r="H52" s="4"/>
     </row>
     <row r="53" spans="1:8">
-      <c r="A53" s="12" t="s">
+      <c r="A53" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B53" s="4">
+        <v>1</v>
+      </c>
+      <c r="C53" s="4">
+        <f>B24/C24</f>
+        <v>0.44395875172476118</v>
+      </c>
+      <c r="D53" s="4">
+        <f>B24/D24</f>
+        <v>0.45755785860087739</v>
+      </c>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
+      <c r="G53" s="4"/>
+      <c r="H53" s="4"/>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B53" s="12">
-        <v>1</v>
-      </c>
-      <c r="C53" s="12">
+      <c r="B54" s="12">
+        <v>1</v>
+      </c>
+      <c r="C54" s="12">
         <v>0.92227567290000001</v>
       </c>
-      <c r="D53" s="4" t="e">
+      <c r="D54" s="4" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E53" s="12"/>
-      <c r="F53" s="12"/>
-      <c r="G53" s="12"/>
-      <c r="H53" s="12"/>
-    </row>
-    <row r="54" spans="1:8">
-      <c r="A54" s="12"/>
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
-      <c r="H54" s="1"/>
+      <c r="E54" s="12"/>
+      <c r="F54" s="12"/>
+      <c r="G54" s="12"/>
+      <c r="H54" s="12"/>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="1"/>
+      <c r="A55" s="12"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
@@ -1607,27 +4474,27 @@
       <c r="H58" s="1"/>
     </row>
     <row r="59" spans="1:8">
-      <c r="A59" s="12"/>
+      <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
-      <c r="F59" s="2"/>
+      <c r="F59" s="1"/>
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
     </row>
     <row r="60" spans="1:8">
-      <c r="A60" s="3"/>
-      <c r="B60" s="4"/>
-      <c r="C60" s="4"/>
-      <c r="D60" s="4"/>
-      <c r="E60" s="4"/>
-      <c r="F60" s="4"/>
-      <c r="G60" s="4"/>
-      <c r="H60" s="4"/>
+      <c r="A60" s="12"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="2"/>
+      <c r="G60" s="1"/>
+      <c r="H60" s="1"/>
     </row>
     <row r="61" spans="1:8">
-      <c r="A61" s="5"/>
+      <c r="A61" s="3"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
       <c r="D61" s="4"/>
@@ -1637,7 +4504,7 @@
       <c r="H61" s="4"/>
     </row>
     <row r="62" spans="1:8">
-      <c r="A62" s="3"/>
+      <c r="A62" s="5"/>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
       <c r="D62" s="4"/>
@@ -1647,7 +4514,7 @@
       <c r="H62" s="4"/>
     </row>
     <row r="63" spans="1:8">
-      <c r="A63" s="5"/>
+      <c r="A63" s="3"/>
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
       <c r="D63" s="4"/>
@@ -1677,7 +4544,7 @@
       <c r="H65" s="4"/>
     </row>
     <row r="66" spans="1:8">
-      <c r="A66" s="3"/>
+      <c r="A66" s="5"/>
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
       <c r="D66" s="4"/>
@@ -1687,7 +4554,7 @@
       <c r="H66" s="4"/>
     </row>
     <row r="67" spans="1:8">
-      <c r="A67" s="5"/>
+      <c r="A67" s="3"/>
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
       <c r="D67" s="4"/>
@@ -1697,7 +4564,7 @@
       <c r="H67" s="4"/>
     </row>
     <row r="68" spans="1:8">
-      <c r="A68" s="3"/>
+      <c r="A68" s="5"/>
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
       <c r="D68" s="4"/>
@@ -1717,7 +4584,7 @@
       <c r="H69" s="4"/>
     </row>
     <row r="70" spans="1:8">
-      <c r="A70" s="5"/>
+      <c r="A70" s="3"/>
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
       <c r="D70" s="4"/>
@@ -1727,7 +4594,7 @@
       <c r="H70" s="4"/>
     </row>
     <row r="71" spans="1:8">
-      <c r="A71" s="3"/>
+      <c r="A71" s="5"/>
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
       <c r="D71" s="4"/>
@@ -1737,7 +4604,7 @@
       <c r="H71" s="4"/>
     </row>
     <row r="72" spans="1:8">
-      <c r="A72" s="6"/>
+      <c r="A72" s="3"/>
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
       <c r="D72" s="4"/>
@@ -1747,7 +4614,7 @@
       <c r="H72" s="4"/>
     </row>
     <row r="73" spans="1:8">
-      <c r="A73" s="7"/>
+      <c r="A73" s="6"/>
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
       <c r="D73" s="4"/>
@@ -1777,18 +4644,18 @@
       <c r="H75" s="4"/>
     </row>
     <row r="76" spans="1:8">
-      <c r="A76" s="1"/>
-      <c r="B76" s="8"/>
-      <c r="C76" s="1"/>
-      <c r="D76" s="1"/>
-      <c r="E76" s="1"/>
-      <c r="F76" s="5"/>
-      <c r="G76" s="1"/>
-      <c r="H76" s="1"/>
+      <c r="A76" s="7"/>
+      <c r="B76" s="4"/>
+      <c r="C76" s="4"/>
+      <c r="D76" s="4"/>
+      <c r="E76" s="4"/>
+      <c r="F76" s="4"/>
+      <c r="G76" s="4"/>
+      <c r="H76" s="4"/>
     </row>
     <row r="77" spans="1:8">
       <c r="A77" s="1"/>
-      <c r="B77" s="1"/>
+      <c r="B77" s="8"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
@@ -1804,17 +4671,17 @@
       <c r="E78" s="1"/>
       <c r="F78" s="5"/>
       <c r="G78" s="1"/>
-      <c r="H78" s="13"/>
+      <c r="H78" s="1"/>
     </row>
     <row r="79" spans="1:8">
-      <c r="A79" s="4"/>
-      <c r="B79" s="4"/>
-      <c r="C79" s="4"/>
-      <c r="D79" s="4"/>
-      <c r="E79" s="4"/>
-      <c r="F79" s="4"/>
-      <c r="G79" s="4"/>
-      <c r="H79" s="4"/>
+      <c r="A79" s="1"/>
+      <c r="B79" s="1"/>
+      <c r="C79" s="1"/>
+      <c r="D79" s="1"/>
+      <c r="E79" s="1"/>
+      <c r="F79" s="5"/>
+      <c r="G79" s="1"/>
+      <c r="H79" s="13"/>
     </row>
     <row r="80" spans="1:8">
       <c r="A80" s="4"/>
@@ -1847,14 +4714,14 @@
       <c r="H82" s="4"/>
     </row>
     <row r="83" spans="1:8">
-      <c r="A83" s="1"/>
-      <c r="B83" s="1"/>
-      <c r="C83" s="1"/>
-      <c r="D83" s="1"/>
-      <c r="E83" s="1"/>
-      <c r="F83" s="1"/>
-      <c r="G83" s="1"/>
-      <c r="H83" s="1"/>
+      <c r="A83" s="4"/>
+      <c r="B83" s="4"/>
+      <c r="C83" s="4"/>
+      <c r="D83" s="4"/>
+      <c r="E83" s="4"/>
+      <c r="F83" s="4"/>
+      <c r="G83" s="4"/>
+      <c r="H83" s="4"/>
     </row>
     <row r="84" spans="1:8">
       <c r="A84" s="1"/>
@@ -1867,27 +4734,27 @@
       <c r="H84" s="1"/>
     </row>
     <row r="85" spans="1:8">
-      <c r="A85" s="14"/>
+      <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
-      <c r="F85" s="2"/>
+      <c r="F85" s="1"/>
       <c r="G85" s="1"/>
       <c r="H85" s="1"/>
     </row>
     <row r="86" spans="1:8">
-      <c r="A86" s="3"/>
-      <c r="B86" s="4"/>
-      <c r="C86" s="4"/>
-      <c r="D86" s="4"/>
-      <c r="E86" s="4"/>
-      <c r="F86" s="4"/>
-      <c r="G86" s="4"/>
-      <c r="H86" s="4"/>
+      <c r="A86" s="14"/>
+      <c r="B86" s="1"/>
+      <c r="C86" s="1"/>
+      <c r="D86" s="1"/>
+      <c r="E86" s="1"/>
+      <c r="F86" s="2"/>
+      <c r="G86" s="1"/>
+      <c r="H86" s="1"/>
     </row>
     <row r="87" spans="1:8">
-      <c r="A87" s="5"/>
+      <c r="A87" s="3"/>
       <c r="B87" s="4"/>
       <c r="C87" s="4"/>
       <c r="D87" s="4"/>
@@ -1897,7 +4764,7 @@
       <c r="H87" s="4"/>
     </row>
     <row r="88" spans="1:8">
-      <c r="A88" s="3"/>
+      <c r="A88" s="5"/>
       <c r="B88" s="4"/>
       <c r="C88" s="4"/>
       <c r="D88" s="4"/>
@@ -1907,7 +4774,7 @@
       <c r="H88" s="4"/>
     </row>
     <row r="89" spans="1:8">
-      <c r="A89" s="5"/>
+      <c r="A89" s="3"/>
       <c r="B89" s="4"/>
       <c r="C89" s="4"/>
       <c r="D89" s="4"/>
@@ -1937,7 +4804,7 @@
       <c r="H91" s="4"/>
     </row>
     <row r="92" spans="1:8">
-      <c r="A92" s="3"/>
+      <c r="A92" s="5"/>
       <c r="B92" s="4"/>
       <c r="C92" s="4"/>
       <c r="D92" s="4"/>
@@ -1947,7 +4814,7 @@
       <c r="H92" s="4"/>
     </row>
     <row r="93" spans="1:8">
-      <c r="A93" s="5"/>
+      <c r="A93" s="3"/>
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
       <c r="D93" s="4"/>
@@ -1957,7 +4824,7 @@
       <c r="H93" s="4"/>
     </row>
     <row r="94" spans="1:8">
-      <c r="A94" s="3"/>
+      <c r="A94" s="5"/>
       <c r="B94" s="4"/>
       <c r="C94" s="4"/>
       <c r="D94" s="4"/>
@@ -1977,7 +4844,7 @@
       <c r="H95" s="4"/>
     </row>
     <row r="96" spans="1:8">
-      <c r="A96" s="5"/>
+      <c r="A96" s="3"/>
       <c r="B96" s="4"/>
       <c r="C96" s="4"/>
       <c r="D96" s="4"/>
@@ -1987,7 +4854,7 @@
       <c r="H96" s="4"/>
     </row>
     <row r="97" spans="1:8">
-      <c r="A97" s="3"/>
+      <c r="A97" s="5"/>
       <c r="B97" s="4"/>
       <c r="C97" s="4"/>
       <c r="D97" s="4"/>
@@ -1997,7 +4864,7 @@
       <c r="H97" s="4"/>
     </row>
     <row r="98" spans="1:8">
-      <c r="A98" s="6"/>
+      <c r="A98" s="3"/>
       <c r="B98" s="4"/>
       <c r="C98" s="4"/>
       <c r="D98" s="4"/>
@@ -2007,7 +4874,7 @@
       <c r="H98" s="4"/>
     </row>
     <row r="99" spans="1:8">
-      <c r="A99" s="7"/>
+      <c r="A99" s="6"/>
       <c r="B99" s="4"/>
       <c r="C99" s="4"/>
       <c r="D99" s="4"/>
@@ -2037,7 +4904,7 @@
       <c r="H101" s="4"/>
     </row>
     <row r="102" spans="1:8">
-      <c r="A102" s="1"/>
+      <c r="A102" s="7"/>
       <c r="B102" s="4"/>
       <c r="C102" s="4"/>
       <c r="D102" s="4"/>
@@ -2057,7 +4924,7 @@
       <c r="H103" s="4"/>
     </row>
     <row r="104" spans="1:8">
-      <c r="A104" s="15"/>
+      <c r="A104" s="1"/>
       <c r="B104" s="4"/>
       <c r="C104" s="4"/>
       <c r="D104" s="4"/>
@@ -2077,7 +4944,7 @@
       <c r="H105" s="4"/>
     </row>
     <row r="106" spans="1:8">
-      <c r="A106" s="4"/>
+      <c r="A106" s="15"/>
       <c r="B106" s="4"/>
       <c r="C106" s="4"/>
       <c r="D106" s="4"/>
@@ -2117,16 +4984,27 @@
       <c r="H109" s="4"/>
     </row>
     <row r="110" spans="1:8">
-      <c r="A110" s="12"/>
-      <c r="B110" s="1"/>
-      <c r="C110" s="1"/>
-      <c r="D110" s="1"/>
-      <c r="E110" s="1"/>
-      <c r="F110" s="1"/>
-      <c r="G110" s="1"/>
-      <c r="H110" s="1"/>
+      <c r="A110" s="4"/>
+      <c r="B110" s="4"/>
+      <c r="C110" s="4"/>
+      <c r="D110" s="4"/>
+      <c r="E110" s="4"/>
+      <c r="F110" s="4"/>
+      <c r="G110" s="4"/>
+      <c r="H110" s="4"/>
+    </row>
+    <row r="111" spans="1:8">
+      <c r="A111" s="12"/>
+      <c r="B111" s="1"/>
+      <c r="C111" s="1"/>
+      <c r="D111" s="1"/>
+      <c r="E111" s="1"/>
+      <c r="F111" s="1"/>
+      <c r="G111" s="1"/>
+      <c r="H111" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>